<commit_message>
add some folder for pfsense
</commit_message>
<xml_diff>
--- a/Phân_công_nhiệm_vụ.xlsx
+++ b/Phân_công_nhiệm_vụ.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="12570"/>
+    <workbookView windowWidth="13785" windowHeight="12270" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="IP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
   <si>
     <t>Phân Công nhiệm vụ thực hiện Project</t>
   </si>
@@ -140,6 +141,48 @@
   </si>
   <si>
     <t>Cấu hình sao cho Home_PC có thể ping được tới các PC trong phòng ban IT.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiết bị </t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP address </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW_Core_A </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vlan 10 </t>
+  </si>
+  <si>
+    <t>192.168.2.65/26</t>
+  </si>
+  <si>
+    <t>Vlan 15</t>
+  </si>
+  <si>
+    <t>192.168.2.1/26</t>
+  </si>
+  <si>
+    <t>Vlan 20</t>
+  </si>
+  <si>
+    <t>192.168.2.145/29</t>
+  </si>
+  <si>
+    <t>Vlan 25</t>
+  </si>
+  <si>
+    <t>192.168.2.129/28</t>
+  </si>
+  <si>
+    <t>e0/1</t>
+  </si>
+  <si>
+    <t>192.168.3.5/25</t>
   </si>
 </sst>
 </file>
@@ -147,12 +190,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +204,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -205,8 +261,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,14 +285,99 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,14 +392,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -258,96 +399,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="41">
     <fill>
@@ -412,181 +468,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -667,17 +723,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -715,15 +767,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -739,13 +782,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -754,152 +810,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="38" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -912,58 +968,70 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1287,534 +1355,534 @@
   <sheetPr/>
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="13.5583333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.225" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.5583333333333" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6333333333333" style="1" customWidth="1"/>
-    <col min="6" max="6" width="51" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="13.5583333333333" style="5" customWidth="1"/>
+    <col min="2" max="2" width="41.75" style="5" customWidth="1"/>
+    <col min="3" max="3" width="34.225" style="5" customWidth="1"/>
+    <col min="4" max="4" width="34.5583333333333" style="5" customWidth="1"/>
+    <col min="5" max="5" width="21.6333333333333" style="5" customWidth="1"/>
+    <col min="6" max="6" width="51" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="21" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="3" spans="5:6">
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="15" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="4"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="21" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="4"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19" t="s">
+      <c r="E7" s="22"/>
+      <c r="F7" s="23" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="5:6">
-      <c r="E8" s="20"/>
-      <c r="F8" s="21" t="s">
+      <c r="E8" s="24"/>
+      <c r="F8" s="25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="10">
+      <c r="A11" s="14">
         <v>1</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="4"/>
+      <c r="E11" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="10">
+      <c r="A12" s="14">
         <v>2</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="4"/>
+      <c r="E12" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="10">
+      <c r="A13" s="14">
         <v>3</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="4"/>
+      <c r="E13" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="10">
+      <c r="A14" s="14">
         <v>4</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="4"/>
+      <c r="E14" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="10">
-        <v>5</v>
-      </c>
-      <c r="B15" s="13" t="s">
+      <c r="A15" s="14">
+        <v>5</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="4"/>
+      <c r="E15" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="10">
+      <c r="A16" s="14">
         <v>6</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="4"/>
+      <c r="E16" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" ht="54" spans="1:6">
-      <c r="A17" s="10">
+      <c r="A17" s="14">
         <v>7</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="4"/>
+      <c r="E17" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="10">
+      <c r="A18" s="14">
         <v>8</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="4"/>
+      <c r="E18" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" ht="54" spans="1:6">
-      <c r="A19" s="10">
+      <c r="A19" s="14">
         <v>9</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="4"/>
+      <c r="E19" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" ht="36" spans="1:6">
-      <c r="A20" s="10">
+      <c r="A20" s="14">
         <v>10</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="4"/>
+      <c r="E20" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" ht="36" spans="1:6">
-      <c r="A21" s="10">
+      <c r="A21" s="14">
         <v>11</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="4"/>
+      <c r="E21" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" ht="54" spans="1:6">
-      <c r="A22" s="10">
+      <c r="A22" s="14">
         <v>12</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="4"/>
+      <c r="E22" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" ht="54" spans="1:6">
-      <c r="A23" s="10">
+      <c r="A23" s="14">
         <v>13</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="4"/>
+      <c r="E23" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="8"/>
     </row>
     <row r="24" ht="54" spans="1:6">
-      <c r="A24" s="10">
+      <c r="A24" s="14">
         <v>14</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="4"/>
+      <c r="E24" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="8"/>
     </row>
     <row r="25" ht="36" spans="1:6">
-      <c r="A25" s="10">
+      <c r="A25" s="14">
         <v>15</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="4"/>
+      <c r="E25" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="8"/>
     </row>
     <row r="26" ht="36" spans="1:6">
-      <c r="A26" s="10">
+      <c r="A26" s="14">
         <v>16</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" s="4"/>
+      <c r="E26" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" ht="54" spans="1:6">
-      <c r="A27" s="10">
+      <c r="A27" s="14">
         <v>17</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="4"/>
+      <c r="E27" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="8"/>
     </row>
     <row r="28" ht="54" spans="1:6">
-      <c r="A28" s="10">
+      <c r="A28" s="14">
         <v>18</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F28" s="4"/>
+      <c r="E28" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="8"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="10">
+      <c r="A29" s="14">
         <v>19</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" s="4"/>
+      <c r="E29" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="8"/>
     </row>
     <row r="30" ht="36" spans="1:6">
-      <c r="A30" s="10">
+      <c r="A30" s="14">
         <v>20</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" s="4"/>
+      <c r="E30" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="8"/>
     </row>
     <row r="31" ht="54" spans="1:6">
-      <c r="A31" s="10">
+      <c r="A31" s="14">
         <v>21</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F31" s="4"/>
+      <c r="E31" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="8"/>
     </row>
     <row r="32" ht="36" spans="1:6">
-      <c r="A32" s="10">
+      <c r="A32" s="14">
         <v>22</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E32" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" s="4"/>
+      <c r="E32" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="8"/>
     </row>
     <row r="33" ht="54" spans="1:6">
-      <c r="A33" s="10">
+      <c r="A33" s="14">
         <v>23</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E33" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" s="4"/>
+      <c r="E33" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1826,4 +1894,88 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="17.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:A7"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>